<commit_message>
fix: correct value type in mapping
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63F151-0033-4C20-9DAD-37D7F5B04D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30103B8F-9BBC-49F4-881C-CCE0485D3566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -772,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -868,9 +868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1002,7 @@
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -1255,7 +1255,7 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1354,7 +1354,7 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -1642,7 +1642,7 @@
         <v>28</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
refactor: added to standard mapping
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30103B8F-9BBC-49F4-881C-CCE0485D3566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C42173-5CB0-46DC-B881-F4DD4D25012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -401,6 +401,18 @@
   </si>
   <si>
     <t>v1.0</t>
+  </si>
+  <si>
+    <t>The CogniteSourceSystem core concept is used to standardize the way source system is stored.</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteDescribable(version=v1)</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteSourceSystem(version=v1)</t>
+  </si>
+  <si>
+    <t>The describable core concept is used as a standard way of holding the bare minimum of information about the instance</t>
   </si>
 </sst>
 </file>
@@ -868,9 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1894,16 +1906,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="73.6640625" customWidth="1"/>
     <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
@@ -2012,11 +2024,37 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: bug in mapping to cognite types
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FFFFB9-F945-4B76-BE82-F9D9AC7CABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11007C1E-956F-498D-9BD2-9A6BC796AD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
   <si>
     <t>role</t>
   </si>
@@ -397,9 +397,6 @@
     <t>cdf_cdm:CogniteTimeSeries(version=v1)</t>
   </si>
   <si>
-    <t>cdf_cdm:SourceSystem(version=v1)</t>
-  </si>
-  <si>
     <t>v1.0</t>
   </si>
   <si>
@@ -410,6 +407,15 @@
   </si>
   <si>
     <t>cdf_cdm:CogniteSourceSystem(version=v1)</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteUnit(version=v1)</t>
+  </si>
+  <si>
+    <t>Represents a single unit of measurement</t>
+  </si>
+  <si>
+    <t>CogniteDescribable</t>
   </si>
 </sst>
 </file>
@@ -785,13 +791,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -807,7 +813,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -815,15 +821,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -831,7 +837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -839,7 +845,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -847,7 +853,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -855,7 +861,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -863,7 +869,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -879,27 +885,27 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="70" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -918,7 +924,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -965,7 +971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1125,7 +1131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1317,7 +1323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1512,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1733,7 +1739,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -1864,7 +1870,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1903,23 +1909,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>86</v>
       </c>
@@ -1930,7 +1936,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1953,7 +1959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2021,17 +2027,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>128</v>
       </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" t="b">
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2053,14 +2073,14 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
@@ -2068,7 +2088,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>95</v>
       </c>
@@ -2082,7 +2102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2096,7 +2116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
🐛Refactor introduced bugs (#786)
* fix: bug in loaders

* fix: bug in mapping to cognite types

* fix: update relationship unpacker

* docs: Why

* feat: remvoe system spaces in DMS export

* fix: stuff

* fix: exclude core in the correct way

* fix: actually remove cdf spaces

* fix; poor implemenation

* fix: include referenced views in data model

* fix: namespace

* fix: bug in relationship unpacker

* feat; better handling of edge soruce

* tests; skip

* build: changelog
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FFFFB9-F945-4B76-BE82-F9D9AC7CABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11007C1E-956F-498D-9BD2-9A6BC796AD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
   <si>
     <t>role</t>
   </si>
@@ -397,9 +397,6 @@
     <t>cdf_cdm:CogniteTimeSeries(version=v1)</t>
   </si>
   <si>
-    <t>cdf_cdm:SourceSystem(version=v1)</t>
-  </si>
-  <si>
     <t>v1.0</t>
   </si>
   <si>
@@ -410,6 +407,15 @@
   </si>
   <si>
     <t>cdf_cdm:CogniteSourceSystem(version=v1)</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteUnit(version=v1)</t>
+  </si>
+  <si>
+    <t>Represents a single unit of measurement</t>
+  </si>
+  <si>
+    <t>CogniteDescribable</t>
   </si>
 </sst>
 </file>
@@ -785,13 +791,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -807,7 +813,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -815,15 +821,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -831,7 +837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -839,7 +845,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -847,7 +853,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -855,7 +861,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -863,7 +869,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -879,27 +885,27 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="70" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -918,7 +924,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -965,7 +971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1125,7 +1131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1317,7 +1323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1491,7 +1497,7 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1512,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1733,7 +1739,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -1864,7 +1870,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1903,23 +1909,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>86</v>
       </c>
@@ -1930,7 +1936,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1953,7 +1959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2021,17 +2027,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>128</v>
       </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" t="b">
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2053,14 +2073,14 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
@@ -2068,7 +2088,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>95</v>
       </c>
@@ -2082,7 +2102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2096,7 +2116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
fix: bug in mapping
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11007C1E-956F-498D-9BD2-9A6BC796AD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2CE7B-EC5E-4A31-AD53-56045E519DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>Represents a single unit of measurement</t>
-  </si>
-  <si>
-    <t>CogniteDescribable</t>
   </si>
 </sst>
 </file>
@@ -791,13 +788,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,7 +810,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -821,7 +818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,7 +826,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -837,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -845,7 +842,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -853,7 +850,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -861,7 +858,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -869,7 +866,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -888,24 +885,24 @@
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="70" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="68.44140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
     <col min="7" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.42578125" customWidth="1"/>
-    <col min="12" max="12" width="37.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.44140625" customWidth="1"/>
+    <col min="12" max="12" width="37.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -924,7 +921,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -971,7 +968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1064,7 +1061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1096,7 +1093,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1192,7 +1189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1288,7 +1285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1387,7 +1384,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1550,7 +1547,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1640,7 +1637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1675,7 +1672,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1739,7 +1736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1803,7 +1800,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1835,7 +1832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1870,7 +1867,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1913,19 +1910,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>86</v>
       </c>
@@ -1936,7 +1933,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1976,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1993,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2010,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -2041,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -2049,7 +2046,7 @@
         <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -2073,14 +2070,14 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
@@ -2088,7 +2085,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>95</v>
       </c>
@@ -2102,7 +2099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2116,7 +2113,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
[NEAT-586] 😧 As parent name (#793)
* refactor; setup interface

* refactor: first draft

* refactor: fix

* fix: bug in mapping

* fix: first working version

* tests: updated test

* tests: no duplicates

* tests: made test trigger bug

* fix: avoid duplicates

* build: changelog

* refactor: review feedback

* tests: fix tests
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11007C1E-956F-498D-9BD2-9A6BC796AD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2CE7B-EC5E-4A31-AD53-56045E519DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>Represents a single unit of measurement</t>
-  </si>
-  <si>
-    <t>CogniteDescribable</t>
   </si>
 </sst>
 </file>
@@ -791,13 +788,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,7 +810,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -821,7 +818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,7 +826,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -837,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -845,7 +842,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -853,7 +850,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -861,7 +858,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -869,7 +866,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -888,24 +885,24 @@
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="70" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="68.44140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
     <col min="7" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.42578125" customWidth="1"/>
-    <col min="12" max="12" width="37.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.44140625" customWidth="1"/>
+    <col min="12" max="12" width="37.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -924,7 +921,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -971,7 +968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1064,7 +1061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1096,7 +1093,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1192,7 +1189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1288,7 +1285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -1387,7 +1384,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1550,7 +1547,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1640,7 +1637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1675,7 +1672,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1739,7 +1736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1803,7 +1800,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1835,7 +1832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1870,7 +1867,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1913,19 +1910,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>86</v>
       </c>
@@ -1936,7 +1933,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1976,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1993,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2010,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -2041,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -2049,7 +2046,7 @@
         <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -2073,14 +2070,14 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
@@ -2088,7 +2085,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>95</v>
       </c>
@@ -2102,7 +2099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2116,7 +2113,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
refactor: mapping to ClasicSourceSystem
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2CE7B-EC5E-4A31-AD53-56045E519DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD28035-BCE1-4DC2-8974-0C7F2ED8219A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="30960" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="131">
   <si>
     <t>role</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>Represents a single unit of measurement</t>
+  </si>
+  <si>
+    <t>ClassicSourceSystem</t>
   </si>
 </sst>
 </file>
@@ -880,9 +883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,7 +1110,7 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -1299,7 +1302,7 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1494,7 +1497,7 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1908,9 +1911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,13 +2029,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
         <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
refactor: added connections to classic core mapping
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D365AE-0DBC-4C47-A06F-6C743F23D709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B12FAE-1825-4BCC-8606-F690056C829B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="173">
   <si>
     <t>role</t>
   </si>
@@ -416,6 +416,132 @@
   </si>
   <si>
     <t>ClassicSourceSystem</t>
+  </si>
+  <si>
+    <t>ClassicEquipment</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteEquipment(version=v1)</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Equipment represents physical supplies or devices.</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>timeSeries</t>
+  </si>
+  <si>
+    <t>A list of equipment the activity is related to.</t>
+  </si>
+  <si>
+    <t>A list of time series the activity is related to.</t>
+  </si>
+  <si>
+    <t>activities</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>An automatically updated list of activities related to the asset.</t>
+  </si>
+  <si>
+    <t>reverse(property=assets)</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>An automatically updated list of assets with this asset as their parent.</t>
+  </si>
+  <si>
+    <t>reverse(property=parent)</t>
+  </si>
+  <si>
+    <t>An automatically updated list of equipment related to the asset.</t>
+  </si>
+  <si>
+    <t>reverse(property=asset)</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>An automatically updated list of files related to the asset.</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>An automatically updated ordered list of this asset's ancestors, starting with the root asset. Enables subtree filtering to find all assets under a parent.</t>
+  </si>
+  <si>
+    <t>assetHierarchy_path</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>An automatically updated reference to the top-level asset of the hierarchy.</t>
+  </si>
+  <si>
+    <t>assetHierarchy_root</t>
+  </si>
+  <si>
+    <t>An automatically updated list of time series related to the asset.</t>
+  </si>
+  <si>
+    <t>An automatically updated list of equipment this file is related to.</t>
+  </si>
+  <si>
+    <t>reverse(property=files)</t>
+  </si>
+  <si>
+    <t>An automatically updated list of activities the time series is related to.</t>
+  </si>
+  <si>
+    <t>reverse(property=timeSeries)</t>
+  </si>
+  <si>
+    <t>A list of equipment the time series is related to.</t>
+  </si>
+  <si>
+    <t>An automatically updated list of activities related to the equipment.</t>
+  </si>
+  <si>
+    <t>reverse(property=equipment)</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>The asset the equipment is related to.</t>
+  </si>
+  <si>
+    <t>cdf_cdm:CogniteEquipment</t>
+  </si>
+  <si>
+    <t>A list of files the equipment relates to.</t>
+  </si>
+  <si>
+    <t>An automatically updated list of time series related to the equipment.</t>
   </si>
 </sst>
 </file>
@@ -881,28 +1007,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L39" sqref="L39"/>
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="70" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="70" customWidth="1"/>
+    <col min="5" max="5" width="68.44140625" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" customWidth="1"/>
-    <col min="7" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" customWidth="1"/>
     <col min="11" max="11" width="36.44140625" customWidth="1"/>
     <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="13" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
@@ -1194,16 +1320,22 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>135</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>137</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1212,27 +1344,33 @@
         <v>0</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="L11" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1241,51 +1379,13 @@
         <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>60</v>
-      </c>
-      <c r="L13" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1293,16 +1393,13 @@
         <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1314,13 +1411,10 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1328,10 +1422,10 @@
         <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
         <v>33</v>
@@ -1343,33 +1437,68 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="s">
         <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="M15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -1378,27 +1507,27 @@
         <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
         <v>33</v>
@@ -1410,190 +1539,125 @@
         <v>0</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>142</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>143</v>
+      </c>
+      <c r="C21" t="s">
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>147</v>
+      </c>
+      <c r="E22" t="s">
+        <v>148</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" t="s">
-        <v>40</v>
-      </c>
-      <c r="M22" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" t="s">
         <v>103</v>
       </c>
-      <c r="B23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
       <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
-        <v>39</v>
-      </c>
-      <c r="L23" t="s">
-        <v>42</v>
-      </c>
-      <c r="M23" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>152</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>154</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -1605,88 +1669,88 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="L24" t="s">
-        <v>44</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" t="s">
         <v>104</v>
       </c>
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
       <c r="I26" t="b">
         <v>1</v>
-      </c>
-      <c r="K26" t="s">
-        <v>34</v>
-      </c>
-      <c r="L26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" t="s">
-        <v>74</v>
-      </c>
-      <c r="L27" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -1695,33 +1759,33 @@
         <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="L28" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -1729,25 +1793,25 @@
       <c r="I29" t="b">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
-        <v>69</v>
-      </c>
       <c r="K29" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
@@ -1762,27 +1826,21 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="L30" t="s">
-        <v>5</v>
-      </c>
-      <c r="M30" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
         <v>33</v>
@@ -1797,132 +1855,722 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="L31" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" t="s">
+        <v>42</v>
+      </c>
+      <c r="M34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
+      </c>
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" t="s">
+        <v>131</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>74</v>
+      </c>
+      <c r="L40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>69</v>
+      </c>
+      <c r="K42" t="s">
+        <v>74</v>
+      </c>
+      <c r="L42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" t="s">
+        <v>5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>74</v>
+      </c>
+      <c r="L44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C45" t="s">
         <v>81</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D45" t="s">
         <v>82</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F45" t="s">
         <v>119</v>
       </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
         <v>74</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>104</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B46" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C46" t="s">
         <v>84</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D46" t="s">
         <v>85</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F46" t="s">
         <v>128</v>
       </c>
-      <c r="G33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
         <v>74</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>104</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B47" t="s">
         <v>109</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D47" t="s">
         <v>45</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F47" t="s">
         <v>33</v>
       </c>
-      <c r="G34" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
         <v>34</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
         <v>130</v>
       </c>
-      <c r="B36" t="s">
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="s">
+        <v>39</v>
+      </c>
+      <c r="L49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" t="s">
+        <v>163</v>
+      </c>
+      <c r="E50" t="s">
+        <v>164</v>
+      </c>
+      <c r="F50" t="s">
+        <v>101</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>74</v>
+      </c>
+      <c r="L51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F53" t="s">
         <v>33</v>
       </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="s">
         <v>34</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L53" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" t="s">
+        <v>140</v>
+      </c>
+      <c r="D55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F55" t="s">
+        <v>101</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="s">
+        <v>170</v>
+      </c>
+      <c r="L56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="s">
+        <v>103</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>170</v>
+      </c>
+      <c r="L57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" t="s">
+        <v>167</v>
+      </c>
+      <c r="F58" t="s">
+        <v>104</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="s">
+        <v>39</v>
+      </c>
+      <c r="L59" t="s">
+        <v>37</v>
+      </c>
+      <c r="M59" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1935,11 +2583,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2053,31 +2701,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>130</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C7" t="s">
         <v>125</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D7" t="s">
         <v>127</v>
       </c>
-      <c r="F8" t="b">
+      <c r="F7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>128</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>126</v>
       </c>
-      <c r="F9" t="b">
+      <c r="F10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor; update excel to yaml script
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B12FAE-1825-4BCC-8606-F690056C829B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BD7886-5794-493D-8FB6-E1F90459B565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1008" windowWidth="23232" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>DMS Architect</t>
   </si>
   <si>
-    <t>prefix</t>
-  </si>
-  <si>
     <t>externalId</t>
   </si>
   <si>
@@ -542,6 +539,9 @@
   </si>
   <si>
     <t>An automatically updated list of time series related to the equipment.</t>
+  </si>
+  <si>
+    <t>space</t>
   </si>
 </sst>
 </file>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,55 +933,55 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>45533.576350648153</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>45533.576350648153</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
@@ -1033,7 +1033,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1052,223 +1052,223 @@
     </row>
     <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
       <c r="L5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>56</v>
-      </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1280,62 +1280,62 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
         <v>56</v>
       </c>
-      <c r="L8" t="s">
-        <v>57</v>
-      </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1347,30 +1347,30 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1382,190 +1382,190 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
         <v>33</v>
       </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>34</v>
-      </c>
       <c r="L14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>33</v>
       </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>34</v>
-      </c>
       <c r="L15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s">
-        <v>102</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
-        <v>60</v>
-      </c>
-      <c r="L16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
         <v>38</v>
       </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>39</v>
-      </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
         <v>33</v>
       </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>34</v>
-      </c>
       <c r="L18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" t="s">
         <v>139</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>140</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>141</v>
       </c>
-      <c r="E20" t="s">
-        <v>142</v>
-      </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1573,22 +1573,22 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" t="s">
         <v>143</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>144</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>145</v>
       </c>
-      <c r="E21" t="s">
-        <v>146</v>
-      </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1596,22 +1596,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s">
         <v>147</v>
       </c>
-      <c r="E22" t="s">
-        <v>148</v>
-      </c>
       <c r="F22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -1619,22 +1619,22 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" t="s">
         <v>102</v>
-      </c>
-      <c r="B23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" t="s">
-        <v>142</v>
-      </c>
-      <c r="F23" t="s">
-        <v>103</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -1642,92 +1642,92 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" t="s">
         <v>152</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>153</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" t="s">
         <v>154</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="s">
-        <v>60</v>
-      </c>
-      <c r="L24" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
         <v>156</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>157</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" t="s">
         <v>158</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L25" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -1735,54 +1735,54 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
         <v>64</v>
       </c>
-      <c r="E28" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="s">
-        <v>65</v>
-      </c>
       <c r="L28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
         <v>66</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>67</v>
       </c>
-      <c r="D29" t="s">
-        <v>68</v>
-      </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1794,27 +1794,27 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
+        <v>64</v>
+      </c>
+      <c r="L29" t="s">
         <v>65</v>
-      </c>
-      <c r="L29" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>71</v>
       </c>
-      <c r="D30" t="s">
-        <v>72</v>
-      </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1826,91 +1826,91 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
         <v>33</v>
       </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" t="s">
-        <v>34</v>
-      </c>
       <c r="L31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
         <v>38</v>
       </c>
-      <c r="E32" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" t="s">
-        <v>130</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
-        <v>39</v>
-      </c>
       <c r="L32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
         <v>40</v>
       </c>
-      <c r="D33" t="s">
-        <v>41</v>
-      </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -1922,27 +1922,27 @@
         <v>0</v>
       </c>
       <c r="K33" t="s">
+        <v>38</v>
+      </c>
+      <c r="L33" t="s">
         <v>39</v>
       </c>
-      <c r="L33" t="s">
-        <v>40</v>
-      </c>
       <c r="M33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -1954,62 +1954,62 @@
         <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
         <v>33</v>
       </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="K35" t="s">
-        <v>34</v>
-      </c>
       <c r="L35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" t="s">
         <v>161</v>
       </c>
-      <c r="E37" t="s">
-        <v>162</v>
-      </c>
       <c r="F37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -2017,112 +2017,112 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
       <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" t="s">
         <v>32</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
         <v>33</v>
       </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="s">
-        <v>34</v>
-      </c>
       <c r="L39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
         <v>73</v>
       </c>
-      <c r="E40" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>74</v>
-      </c>
       <c r="L40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
         <v>33</v>
       </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" t="s">
-        <v>34</v>
-      </c>
       <c r="L41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" t="s">
         <v>75</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>76</v>
       </c>
-      <c r="D42" t="s">
-        <v>77</v>
-      </c>
       <c r="F42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
@@ -2134,62 +2134,62 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K42" t="s">
+        <v>73</v>
+      </c>
+      <c r="L42" t="s">
         <v>74</v>
-      </c>
-      <c r="L42" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
         <v>33</v>
       </c>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" t="s">
-        <v>34</v>
-      </c>
       <c r="L43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" t="s">
         <v>79</v>
       </c>
-      <c r="D44" t="s">
-        <v>80</v>
-      </c>
       <c r="F44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -2201,27 +2201,27 @@
         <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" t="s">
         <v>81</v>
       </c>
-      <c r="D45" t="s">
-        <v>82</v>
-      </c>
       <c r="F45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
@@ -2233,30 +2233,30 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
         <v>84</v>
       </c>
-      <c r="D46" t="s">
-        <v>85</v>
-      </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -2268,94 +2268,94 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
         <v>33</v>
       </c>
-      <c r="G47" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" t="s">
-        <v>34</v>
-      </c>
       <c r="L47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" t="s">
         <v>37</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="s">
         <v>38</v>
       </c>
-      <c r="E49" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" t="s">
-        <v>130</v>
-      </c>
-      <c r="G49" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="K49" t="s">
-        <v>39</v>
-      </c>
       <c r="L49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" t="s">
         <v>139</v>
       </c>
-      <c r="C50" t="s">
-        <v>140</v>
-      </c>
       <c r="D50" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" t="s">
         <v>163</v>
       </c>
-      <c r="E50" t="s">
-        <v>164</v>
-      </c>
       <c r="F50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I50" t="b">
         <v>1</v>
@@ -2363,22 +2363,22 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -2390,56 +2390,56 @@
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="s">
         <v>33</v>
       </c>
-      <c r="G53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" t="b">
-        <v>0</v>
-      </c>
-      <c r="K53" t="s">
-        <v>34</v>
-      </c>
       <c r="L53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B55" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" t="s">
         <v>139</v>
       </c>
-      <c r="C55" t="s">
-        <v>140</v>
-      </c>
       <c r="D55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E55" t="s">
         <v>166</v>
       </c>
-      <c r="E55" t="s">
-        <v>167</v>
-      </c>
       <c r="F55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I55" t="b">
         <v>1</v>
@@ -2447,57 +2447,57 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
         <v>168</v>
       </c>
-      <c r="C56" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="s">
         <v>169</v>
       </c>
-      <c r="E56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" t="s">
-        <v>102</v>
-      </c>
-      <c r="G56" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" t="s">
-        <v>170</v>
-      </c>
       <c r="L56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" t="s">
         <v>149</v>
       </c>
-      <c r="C57" t="s">
-        <v>150</v>
-      </c>
       <c r="D57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -2509,30 +2509,30 @@
         <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I58" t="b">
         <v>1</v>
@@ -2540,37 +2540,37 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" t="s">
         <v>37</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="s">
         <v>38</v>
       </c>
-      <c r="E59" t="s">
-        <v>28</v>
-      </c>
-      <c r="F59" t="s">
-        <v>130</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" t="b">
-        <v>0</v>
-      </c>
-      <c r="K59" t="s">
-        <v>39</v>
-      </c>
       <c r="L59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2601,7 +2601,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2612,39 +2612,39 @@
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -2652,16 +2652,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -2686,16 +2686,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -2703,13 +2703,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -2717,16 +2717,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
         <v>131</v>
-      </c>
-      <c r="B9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" t="s">
-        <v>132</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
         <v>128</v>
       </c>
-      <c r="C10" t="s">
-        <v>129</v>
-      </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -2773,7 +2773,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2781,44 +2781,44 @@
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refacotor added dummy property
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BD7886-5794-493D-8FB6-E1F90459B565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E9BC3-0A33-4643-A30F-32B00F1689A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1008" windowWidth="23232" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Views" sheetId="3" r:id="rId3"/>
-    <sheet name="Enum" sheetId="5" r:id="rId4"/>
+    <sheet name="Containers" sheetId="6" r:id="rId4"/>
+    <sheet name="Enum" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="179">
   <si>
     <t>role</t>
   </si>
@@ -542,6 +543,24 @@
   </si>
   <si>
     <t>space</t>
+  </si>
+  <si>
+    <t>classicEquipmentGUID</t>
+  </si>
+  <si>
+    <t>Definition of Containers</t>
+  </si>
+  <si>
+    <t>Used For</t>
+  </si>
+  <si>
+    <t>Neat ID</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/neatId_bb7e4121_bc17_46c7_a93d_c855f710ccbe</t>
+  </si>
+  <si>
+    <t>node</t>
   </si>
 </sst>
 </file>
@@ -600,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -609,6 +628,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -1007,11 +1030,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2573,6 +2596,32 @@
         <v>36</v>
       </c>
     </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>173</v>
+      </c>
+      <c r="F60" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="s">
+        <v>130</v>
+      </c>
+      <c r="L60" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
@@ -2587,7 +2636,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomLeft" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2756,6 +2805,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F1C07F-A0DA-4BBF-8751-C8BB96EAA96F}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix: added guid to source system
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E9BC3-0A33-4643-A30F-32B00F1689A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEB8E32-3627-449C-9E13-CA80B5590424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="180">
   <si>
     <t>role</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>node</t>
+  </si>
+  <si>
+    <t>ClassicSourceSystemGUID</t>
   </si>
 </sst>
 </file>
@@ -625,13 +628,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,13 +943,13 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -962,7 +965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -970,7 +973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -978,7 +981,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -986,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -994,7 +997,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1030,50 +1033,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
-    <col min="11" max="11" width="36.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>101</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -2445,82 +2448,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" t="s">
-        <v>138</v>
-      </c>
-      <c r="C55" t="s">
-        <v>139</v>
-      </c>
-      <c r="D55" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" t="s">
-        <v>166</v>
-      </c>
-      <c r="F55" t="s">
-        <v>100</v>
-      </c>
-      <c r="I55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>179</v>
+      </c>
+      <c r="F54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="s">
+        <v>129</v>
+      </c>
+      <c r="L54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="F56" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" t="s">
-        <v>169</v>
-      </c>
-      <c r="L56" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="D57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E57" t="s">
         <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -2529,96 +2523,131 @@
         <v>0</v>
       </c>
       <c r="I57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" t="s">
         <v>169</v>
       </c>
       <c r="L57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E58" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="F58" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
       </c>
       <c r="I58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K58" t="s">
+        <v>169</v>
+      </c>
+      <c r="L58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>135</v>
+      </c>
+      <c r="C59" t="s">
+        <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="F59" t="s">
-        <v>129</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" t="b">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
-      </c>
-      <c r="K59" t="s">
-        <v>38</v>
-      </c>
-      <c r="L59" t="s">
-        <v>36</v>
-      </c>
-      <c r="M59" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>130</v>
       </c>
       <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="s">
+        <v>38</v>
+      </c>
+      <c r="L60" t="s">
+        <v>36</v>
+      </c>
+      <c r="M60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" t="s">
         <v>173</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>32</v>
       </c>
-      <c r="G60" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" t="b">
-        <v>0</v>
-      </c>
-      <c r="K60" t="s">
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
         <v>130</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L61" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2639,27 +2668,27 @@
       <selection pane="bottomLeft" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2682,7 +2711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -2716,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2733,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -2750,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -2764,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -2781,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2806,30 +2835,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F1C07F-A0DA-4BBF-8751-C8BB96EAA96F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2849,7 +2878,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2858,6 +2887,14 @@
       </c>
       <c r="F3" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2874,22 +2911,22 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>94</v>
       </c>
@@ -2903,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2917,7 +2954,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
fix: explicit on guid
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEB8E32-3627-449C-9E13-CA80B5590424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E84798A-82DD-4C5D-9A15-68B1BD321F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
     <t>node</t>
   </si>
   <si>
-    <t>ClassicSourceSystemGUID</t>
+    <t>classicSourceSystemGUID</t>
   </si>
 </sst>
 </file>
@@ -1035,9 +1035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,15 +2665,15 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G10"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2837,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F1C07F-A0DA-4BBF-8751-C8BB96EAA96F}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[NEAT-671] 😃 Add GUID to source system (#891)
* fix: added guid to source system

* tests; regen

* fix: explicit on guid

* refactor: camel case

* refactro: regen

* build: changelog
</commit_message>
<xml_diff>
--- a/scripts/core_classic_mapping.xlsx
+++ b/scripts/core_classic_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E9BC3-0A33-4643-A30F-32B00F1689A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E84798A-82DD-4C5D-9A15-68B1BD321F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="180">
   <si>
     <t>role</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>node</t>
+  </si>
+  <si>
+    <t>classicSourceSystemGUID</t>
   </si>
 </sst>
 </file>
@@ -625,13 +628,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,13 +943,13 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -962,7 +965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -970,7 +973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -978,7 +981,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -986,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -994,7 +997,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>45533.576350648153</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1030,50 +1033,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
-    <col min="11" max="11" width="36.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>101</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -2445,82 +2448,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" t="s">
-        <v>138</v>
-      </c>
-      <c r="C55" t="s">
-        <v>139</v>
-      </c>
-      <c r="D55" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" t="s">
-        <v>166</v>
-      </c>
-      <c r="F55" t="s">
-        <v>100</v>
-      </c>
-      <c r="I55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>179</v>
+      </c>
+      <c r="F54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="s">
+        <v>129</v>
+      </c>
+      <c r="L54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="F56" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" t="s">
-        <v>169</v>
-      </c>
-      <c r="L56" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="D57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E57" t="s">
         <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -2529,96 +2523,131 @@
         <v>0</v>
       </c>
       <c r="I57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" t="s">
         <v>169</v>
       </c>
       <c r="L57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E58" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="F58" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
       </c>
       <c r="I58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K58" t="s">
+        <v>169</v>
+      </c>
+      <c r="L58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>135</v>
+      </c>
+      <c r="C59" t="s">
+        <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="F59" t="s">
-        <v>129</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" t="b">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
-      </c>
-      <c r="K59" t="s">
-        <v>38</v>
-      </c>
-      <c r="L59" t="s">
-        <v>36</v>
-      </c>
-      <c r="M59" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>130</v>
       </c>
       <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="s">
+        <v>38</v>
+      </c>
+      <c r="L60" t="s">
+        <v>36</v>
+      </c>
+      <c r="M60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" t="s">
         <v>173</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>32</v>
       </c>
-      <c r="G60" t="b">
-        <v>1</v>
-      </c>
-      <c r="H60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" t="b">
-        <v>0</v>
-      </c>
-      <c r="K60" t="s">
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
         <v>130</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L61" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2636,30 +2665,30 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G10"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="91.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2682,7 +2711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -2716,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2733,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -2750,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -2764,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -2781,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2806,30 +2835,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F1C07F-A0DA-4BBF-8751-C8BB96EAA96F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2849,7 +2878,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2858,6 +2887,14 @@
       </c>
       <c r="F3" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2874,22 +2911,22 @@
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>94</v>
       </c>
@@ -2903,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2917,7 +2954,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>

</xml_diff>